<commit_message>
this is kapse son changes and grandiose changes
</commit_message>
<xml_diff>
--- a/GRANDIOSE/Memory Mapping.xlsx
+++ b/GRANDIOSE/Memory Mapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="37">
   <si>
     <t>Station-1</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>? For Ideal</t>
+  </si>
+  <si>
+    <t>What about scanned data?</t>
   </si>
 </sst>
 </file>
@@ -210,10 +213,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,7 +489,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,18 +515,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="G2" s="8" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -596,7 +599,7 @@
       <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="G6" s="5"/>
@@ -620,7 +623,9 @@
       <c r="G7" s="3"/>
       <c r="H7" s="5"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="5"/>
+      <c r="J7" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="3">

</xml_diff>